<commit_message>
Add location to database
</commit_message>
<xml_diff>
--- a/评分表.xlsx
+++ b/评分表.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wky/Desktop/Onstagram/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{55980E2E-4C4A-2644-910C-A031B5D4D032}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57284B9-C380-4D47-AF09-B13790EB697A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="720" windowWidth="28040" windowHeight="16140" xr2:uid="{6D5EFA92-2AF3-3B4D-ACF1-42749421FFE6}"/>
+    <workbookView xWindow="3000" yWindow="440" windowWidth="28040" windowHeight="16140" xr2:uid="{6D5EFA92-2AF3-3B4D-ACF1-42749421FFE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>Completed</t>
   </si>
   <si>
-    <t>Sort by location</t>
-  </si>
-  <si>
     <t>Search for user</t>
   </si>
   <si>
@@ -76,6 +73,9 @@
   </si>
   <si>
     <t>附近的人</t>
+  </si>
+  <si>
+    <t>Sort by location and time</t>
   </si>
 </sst>
 </file>
@@ -452,7 +452,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -484,7 +484,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
@@ -492,7 +492,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
@@ -500,7 +500,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="3">
         <v>1</v>
@@ -508,7 +508,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="3">
         <v>3</v>
@@ -516,7 +516,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="3">
         <v>2</v>
@@ -524,7 +524,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="3">
         <v>1</v>
@@ -532,7 +532,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="3">
         <v>1</v>
@@ -540,7 +540,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="3">
         <v>1</v>
@@ -548,7 +548,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="3">
         <v>3</v>
@@ -556,7 +556,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="3">
         <v>2</v>
@@ -564,7 +564,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="3">
         <v>2</v>
@@ -572,7 +572,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="3">
         <v>1</v>
@@ -580,7 +580,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="3">
         <v>4</v>

</xml_diff>

<commit_message>
Add change profile pic
</commit_message>
<xml_diff>
--- a/评分表.xlsx
+++ b/评分表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wky/Desktop/Onstagram/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C2ED8C-F8A3-4F4D-918F-7A5030997CC9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3520E19E-CCEA-504E-B01A-04CA9F5B769B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3000" yWindow="440" windowWidth="28040" windowHeight="16140" xr2:uid="{6D5EFA92-2AF3-3B4D-ACF1-42749421FFE6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Error handlle</t>
   </si>
@@ -458,7 +458,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -586,6 +586,9 @@
       <c r="B14" s="3">
         <v>1</v>
       </c>
+      <c r="C14" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">

</xml_diff>

<commit_message>
Add flash mode, app icon
</commit_message>
<xml_diff>
--- a/评分表.xlsx
+++ b/评分表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wky/Desktop/Onstagram/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E03104-3651-F04D-8758-6FECAAA7499A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B032BE31-E083-5F4A-B7DB-05EE65C41A09}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3000" yWindow="440" windowWidth="28040" windowHeight="16140" xr2:uid="{6D5EFA92-2AF3-3B4D-ACF1-42749421FFE6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>Error handlle</t>
   </si>
@@ -461,7 +461,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -490,6 +490,9 @@
       <c r="B2" s="3">
         <v>1</v>
       </c>
+      <c r="C2" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -509,6 +512,9 @@
       <c r="B4" s="3">
         <v>1</v>
       </c>
+      <c r="C4" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -517,6 +523,9 @@
       <c r="B5" s="3">
         <v>1</v>
       </c>
+      <c r="C5" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -532,6 +541,9 @@
       </c>
       <c r="B7" s="3">
         <v>2</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Add grid on taking photo
</commit_message>
<xml_diff>
--- a/评分表.xlsx
+++ b/评分表.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wky/Desktop/Onstagram/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B032BE31-E083-5F4A-B7DB-05EE65C41A09}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CDE47AD-E503-3E49-AF22-BD82A0086543}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="440" windowWidth="28040" windowHeight="16140" xr2:uid="{6D5EFA92-2AF3-3B4D-ACF1-42749421FFE6}"/>
+    <workbookView xWindow="1000" yWindow="440" windowWidth="28040" windowHeight="16140" xr2:uid="{6D5EFA92-2AF3-3B4D-ACF1-42749421FFE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>Error handlle</t>
   </si>
@@ -461,7 +461,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -553,6 +553,9 @@
       <c r="B8" s="3">
         <v>1</v>
       </c>
+      <c r="C8" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">

</xml_diff>

<commit_message>
Add suggestion algorithm, fix sign up bug
</commit_message>
<xml_diff>
--- a/评分表.xlsx
+++ b/评分表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wky/Desktop/Onstagram/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AFB7AF4-67BA-5845-BE42-7076F16B1643}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1007DFEB-F3BC-D745-8002-4E1EB0A073C7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="440" windowWidth="28040" windowHeight="16140" xr2:uid="{6D5EFA92-2AF3-3B4D-ACF1-42749421FFE6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>Error handlle</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>hide text field</t>
+  </si>
+  <si>
+    <t>signup bug</t>
   </si>
 </sst>
 </file>
@@ -458,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39AC6915-2FA0-E34A-8AC8-3381E65497A0}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -553,6 +556,9 @@
       <c r="B8" s="3">
         <v>1</v>
       </c>
+      <c r="C8" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
@@ -619,6 +625,11 @@
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on user nearby
</commit_message>
<xml_diff>
--- a/评分表.xlsx
+++ b/评分表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wky/Desktop/Onstagram/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1007DFEB-F3BC-D745-8002-4E1EB0A073C7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F988A8E-2646-B44C-A1B9-3455ADC5FBDB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="440" windowWidth="28040" windowHeight="16140" xr2:uid="{6D5EFA92-2AF3-3B4D-ACF1-42749421FFE6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>Error handlle</t>
   </si>
@@ -464,7 +464,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -537,6 +537,9 @@
       <c r="B6" s="3">
         <v>3</v>
       </c>
+      <c r="C6" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -627,9 +630,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>19</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add find nearby users
</commit_message>
<xml_diff>
--- a/评分表.xlsx
+++ b/评分表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wky/Desktop/Onstagram/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F988A8E-2646-B44C-A1B9-3455ADC5FBDB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA4E3FE-93BF-4F41-9FB1-7861BA636239}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="440" windowWidth="28040" windowHeight="16140" xr2:uid="{6D5EFA92-2AF3-3B4D-ACF1-42749421FFE6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>Error handlle</t>
   </si>
@@ -624,6 +624,9 @@
       <c r="B15" s="3">
         <v>4</v>
       </c>
+      <c r="C15" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">

</xml_diff>